<commit_message>
Added Department Model, added freeze, excel sheet download and some changes in routes and auth
</commit_message>
<xml_diff>
--- a/upload/Faculty.xlsx
+++ b/upload/Faculty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WEB DEV\OELP\Sample Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29B520D-1CC8-4983-ABF2-DD1A4F90F560}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9143CE88-1708-4671-96CB-47D0D8315D43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>course13</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>EE</t>
   </si>
 </sst>
 </file>
@@ -457,20 +472,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +496,11 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -492,8 +511,11 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -504,8 +526,11 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -516,8 +541,11 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -528,8 +556,11 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -540,8 +571,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -552,8 +586,11 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -564,8 +601,11 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -576,8 +616,11 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -588,8 +631,11 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -600,8 +646,11 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -611,8 +660,11 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -622,8 +674,11 @@
       <c r="C13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -633,8 +688,11 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -644,8 +702,11 @@
       <c r="C15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
   </sheetData>

</xml_diff>